<commit_message>
update negativa for lectura
</commit_message>
<xml_diff>
--- a/PdfToExcel_Parametros.xlsx
+++ b/PdfToExcel_Parametros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EterEnergy_PdfToExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86856DE7-BB50-4C0C-A7A9-6FEEBB922C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A899E30-77AC-42D4-8EDA-396A1C0E2979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="186">
   <si>
     <t>Selector</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -634,6 +634,9 @@
   </si>
   <si>
     <t>Activa xYYx: xYYxConsumo xYYxdel xYYxperiodo xYYx(Real) xYYxhastaxYYx&amp;&amp;Activa xYYx: xYYxConsumo xYYxdel xYYxperiodo xYYx(Estimada) xYYxhastaxYYx&amp;&amp;Consum xYYxdel xYYxperíode xYYx(Real) xYYxfins&amp;&amp;Consum xYYxdel xYYxperíode xYYx(Estimado) xYYxfins&amp;&amp;Consum xYYxdel xYYxperiodo xYYx(Estimado) xYYxhasta&amp;&amp;Consumo del periodo (Real) hastaxYYx&amp;&amp;Consum del període (Real) fins axYYx&amp;&amp;Consumo del periodo (Estimado) hastaxYYx</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -5014,8 +5017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFBECD2-99BF-47E1-9785-39A18FE51D4F}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -6038,8 +6041,12 @@
       <c r="E61" s="1">
         <v>0</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="F61" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
       <c r="J61" s="1"/>
@@ -6058,8 +6065,12 @@
       <c r="E62" s="1">
         <v>1</v>
       </c>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
@@ -6078,8 +6089,12 @@
       <c r="E63" s="1">
         <v>2</v>
       </c>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="F63" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -6137,8 +6152,12 @@
       <c r="E67" s="1">
         <v>0</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
+      <c r="F67" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
       <c r="J67" s="1"/>
@@ -6157,8 +6176,12 @@
       <c r="E68" s="1">
         <v>1</v>
       </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="F68" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
       <c r="J68" s="1"/>
@@ -6177,8 +6200,12 @@
       <c r="E69" s="1">
         <v>2</v>
       </c>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
       <c r="J69" s="1"/>

</xml_diff>

<commit_message>
Update fix endesa trouble.
</commit_message>
<xml_diff>
--- a/PdfToExcel_Parametros.xlsx
+++ b/PdfToExcel_Parametros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EterEnergy_PdfToExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A899E30-77AC-42D4-8EDA-396A1C0E2979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398329D8-FF60-469F-B71F-42229C65C7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="endesa" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="185">
   <si>
     <t>Selector</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,10 +65,6 @@
     <t>Fecha emisión factura</t>
   </si>
   <si>
-    <t>Total</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>€</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -507,9 +503,6 @@
     <t>Descuentos</t>
   </si>
   <si>
-    <t>TxRx+UxRx</t>
-  </si>
-  <si>
     <t>Factura</t>
   </si>
   <si>
@@ -630,13 +623,16 @@
     <t>TOTAL FACTURAxYYx&amp;&amp;Cese anticipadoxYYx</t>
   </si>
   <si>
-    <t>VxRx+WxRx+XxRx+YxRx+ZxRx+AAxRx-ABxRx</t>
-  </si>
-  <si>
     <t>Activa xYYx: xYYxConsumo xYYxdel xYYxperiodo xYYx(Real) xYYxhastaxYYx&amp;&amp;Activa xYYx: xYYxConsumo xYYxdel xYYxperiodo xYYx(Estimada) xYYxhastaxYYx&amp;&amp;Consum xYYxdel xYYxperíode xYYx(Real) xYYxfins&amp;&amp;Consum xYYxdel xYYxperíode xYYx(Estimado) xYYxfins&amp;&amp;Consum xYYxdel xYYxperiodo xYYx(Estimado) xYYxhasta&amp;&amp;Consumo del periodo (Real) hastaxYYx&amp;&amp;Consum del període (Real) fins axYYx&amp;&amp;Consumo del periodo (Estimado) hastaxYYx</t>
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>VxRx+WxRx+XxRx+YxRx+ZxRx+AAxRx+ABxRx</t>
+  </si>
+  <si>
+    <t>TxRx+VxRx+WxRx+XxRx+YxRx+ZxRx+AAxRx+ABxRx</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1357,7 +1353,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1366,46 +1362,46 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1413,50 +1409,50 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
         <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1464,19 +1460,19 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1484,47 +1480,38 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="K12" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1532,12 +1519,12 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K19" t="s">
         <v>183</v>
@@ -1545,16 +1532,16 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1562,36 +1549,24 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="K21" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1599,16 +1574,16 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1616,31 +1591,31 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1648,16 +1623,16 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1665,13 +1640,13 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -1682,13 +1657,13 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30">
         <v>5</v>
@@ -1699,13 +1674,13 @@
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31">
         <v>5</v>
@@ -1716,158 +1691,158 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1878,13 +1853,13 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -1895,13 +1870,13 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -1912,28 +1887,28 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -1944,13 +1919,13 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68">
         <v>2</v>
@@ -1961,13 +1936,13 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69">
         <v>2</v>
@@ -1978,107 +1953,107 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2114,7 +2089,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2123,33 +2098,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2161,7 +2136,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2173,7 +2148,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2182,7 +2157,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -2191,7 +2166,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2205,10 +2180,10 @@
     </row>
     <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2222,7 +2197,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -2231,16 +2206,16 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -2253,10 +2228,10 @@
     </row>
     <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -2269,13 +2244,13 @@
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -2289,13 +2264,13 @@
     </row>
     <row r="11" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -2309,16 +2284,16 @@
     </row>
     <row r="12" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -2334,7 +2309,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -2348,7 +2323,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -2362,7 +2337,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
@@ -2376,7 +2351,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
@@ -2390,10 +2365,10 @@
     </row>
     <row r="17" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -2411,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -2424,16 +2399,16 @@
     </row>
     <row r="19" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
@@ -2447,22 +2422,22 @@
     </row>
     <row r="20" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -2474,16 +2449,16 @@
     </row>
     <row r="21" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -2499,7 +2474,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
@@ -2513,7 +2488,7 @@
     </row>
     <row r="23" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
@@ -2527,7 +2502,7 @@
     </row>
     <row r="24" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="1"/>
@@ -2541,7 +2516,7 @@
     </row>
     <row r="25" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1"/>
@@ -2555,7 +2530,7 @@
     </row>
     <row r="26" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
@@ -2569,7 +2544,7 @@
     </row>
     <row r="27" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
@@ -2583,7 +2558,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
@@ -2597,13 +2572,13 @@
     </row>
     <row r="29" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2617,13 +2592,13 @@
     </row>
     <row r="30" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1">
         <v>1</v>
@@ -2637,13 +2612,13 @@
     </row>
     <row r="31" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D31" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1">
         <v>1</v>
@@ -2657,7 +2632,7 @@
     </row>
     <row r="32" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -2670,7 +2645,7 @@
     </row>
     <row r="33" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -2683,7 +2658,7 @@
     </row>
     <row r="34" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -2696,7 +2671,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="1"/>
@@ -2710,7 +2685,7 @@
     </row>
     <row r="36" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="1"/>
@@ -2724,7 +2699,7 @@
     </row>
     <row r="37" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A37" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="1"/>
@@ -2738,7 +2713,7 @@
     </row>
     <row r="38" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A38" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="1"/>
@@ -2752,7 +2727,7 @@
     </row>
     <row r="39" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2765,7 +2740,7 @@
     </row>
     <row r="40" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -2778,7 +2753,7 @@
     </row>
     <row r="41" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2791,7 +2766,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -2804,7 +2779,7 @@
     </row>
     <row r="43" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2817,7 +2792,7 @@
     </row>
     <row r="44" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2830,7 +2805,7 @@
     </row>
     <row r="45" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A45" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2843,7 +2818,7 @@
     </row>
     <row r="46" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2856,7 +2831,7 @@
     </row>
     <row r="47" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -2869,7 +2844,7 @@
     </row>
     <row r="48" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2882,7 +2857,7 @@
     </row>
     <row r="49" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A49" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2895,7 +2870,7 @@
     </row>
     <row r="50" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -2908,7 +2883,7 @@
     </row>
     <row r="51" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -2921,7 +2896,7 @@
     </row>
     <row r="52" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A52" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -2934,7 +2909,7 @@
     </row>
     <row r="53" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -2947,7 +2922,7 @@
     </row>
     <row r="54" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A54" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -2960,7 +2935,7 @@
     </row>
     <row r="55" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A55" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -2973,7 +2948,7 @@
     </row>
     <row r="56" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -2986,7 +2961,7 @@
     </row>
     <row r="57" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A57" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -2999,7 +2974,7 @@
     </row>
     <row r="58" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A58" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -3012,7 +2987,7 @@
     </row>
     <row r="59" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A59" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -3025,7 +3000,7 @@
     </row>
     <row r="60" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A60" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -3038,13 +3013,13 @@
     </row>
     <row r="61" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A61" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D61" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1">
         <v>2</v>
@@ -3058,13 +3033,13 @@
     </row>
     <row r="62" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A62" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D62" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62" s="1">
         <v>2</v>
@@ -3078,13 +3053,13 @@
     </row>
     <row r="63" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A63" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D63" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63" s="1">
         <v>2</v>
@@ -3098,7 +3073,7 @@
     </row>
     <row r="64" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A64" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -3111,7 +3086,7 @@
     </row>
     <row r="65" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A65" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -3124,7 +3099,7 @@
     </row>
     <row r="66" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A66" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -3137,13 +3112,13 @@
     </row>
     <row r="67" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A67" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67" s="1">
         <v>2</v>
@@ -3157,13 +3132,13 @@
     </row>
     <row r="68" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A68" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" s="1">
         <v>2</v>
@@ -3177,13 +3152,13 @@
     </row>
     <row r="69" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A69" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D69" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
@@ -3197,7 +3172,7 @@
     </row>
     <row r="70" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A70" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -3210,7 +3185,7 @@
     </row>
     <row r="71" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A71" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -3223,7 +3198,7 @@
     </row>
     <row r="72" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A72" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -3236,7 +3211,7 @@
     </row>
     <row r="73" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A73" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -3249,7 +3224,7 @@
     </row>
     <row r="74" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A74" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -3262,7 +3237,7 @@
     </row>
     <row r="75" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A75" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -3275,7 +3250,7 @@
     </row>
     <row r="76" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A76" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -3288,7 +3263,7 @@
     </row>
     <row r="77" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A77" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -3301,7 +3276,7 @@
     </row>
     <row r="78" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A78" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -3314,7 +3289,7 @@
     </row>
     <row r="79" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A79" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3327,7 +3302,7 @@
     </row>
     <row r="80" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A80" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -3340,7 +3315,7 @@
     </row>
     <row r="81" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A81" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -3353,7 +3328,7 @@
     </row>
     <row r="82" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A82" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -3366,7 +3341,7 @@
     </row>
     <row r="83" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A83" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -3379,7 +3354,7 @@
     </row>
     <row r="84" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A84" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -3392,7 +3367,7 @@
     </row>
     <row r="85" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A85" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -3405,7 +3380,7 @@
     </row>
     <row r="86" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A86" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -3418,7 +3393,7 @@
     </row>
     <row r="87" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A87" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -3431,7 +3406,7 @@
     </row>
     <row r="88" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A88" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -3444,7 +3419,7 @@
     </row>
     <row r="89" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A89" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -3457,7 +3432,7 @@
     </row>
     <row r="90" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A90" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -3495,7 +3470,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3504,33 +3479,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -3542,7 +3517,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -3554,7 +3529,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -3563,7 +3538,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -3572,10 +3547,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
@@ -3588,10 +3563,10 @@
     </row>
     <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -3603,7 +3578,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -3612,13 +3587,13 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -3634,10 +3609,10 @@
     </row>
     <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -3650,13 +3625,13 @@
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -3670,13 +3645,13 @@
     </row>
     <row r="11" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -3690,16 +3665,16 @@
     </row>
     <row r="12" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -3713,7 +3688,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -3727,7 +3702,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -3741,7 +3716,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
@@ -3755,7 +3730,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
@@ -3769,10 +3744,10 @@
     </row>
     <row r="17" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -3790,10 +3765,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1">
         <v>0</v>
@@ -3807,7 +3782,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -3817,21 +3792,21 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
@@ -3845,16 +3820,16 @@
     </row>
     <row r="21" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -3868,16 +3843,16 @@
     </row>
     <row r="22" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
@@ -3891,16 +3866,16 @@
     </row>
     <row r="23" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
@@ -3914,13 +3889,13 @@
     </row>
     <row r="24" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -3930,16 +3905,16 @@
     </row>
     <row r="25" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
         <v>0</v>
@@ -3953,16 +3928,16 @@
     </row>
     <row r="26" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
@@ -3976,16 +3951,16 @@
     </row>
     <row r="27" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
@@ -3999,7 +3974,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
@@ -4013,13 +3988,13 @@
     </row>
     <row r="29" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="1">
         <v>3</v>
@@ -4035,13 +4010,13 @@
     </row>
     <row r="30" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1">
         <v>3</v>
@@ -4057,13 +4032,13 @@
     </row>
     <row r="31" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1">
         <v>3</v>
@@ -4079,13 +4054,13 @@
     </row>
     <row r="32" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E32" s="1">
         <v>3</v>
@@ -4101,13 +4076,13 @@
     </row>
     <row r="33" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E33" s="1">
         <v>3</v>
@@ -4123,13 +4098,13 @@
     </row>
     <row r="34" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E34" s="1">
         <v>3</v>
@@ -4145,42 +4120,42 @@
     </row>
     <row r="35" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A37" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A38" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -4193,7 +4168,7 @@
     </row>
     <row r="41" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -4206,7 +4181,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -4219,7 +4194,7 @@
     </row>
     <row r="43" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -4232,7 +4207,7 @@
     </row>
     <row r="44" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -4245,7 +4220,7 @@
     </row>
     <row r="45" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A45" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -4258,7 +4233,7 @@
     </row>
     <row r="46" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -4271,7 +4246,7 @@
     </row>
     <row r="47" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -4284,7 +4259,7 @@
     </row>
     <row r="48" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -4297,7 +4272,7 @@
     </row>
     <row r="49" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A49" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -4310,7 +4285,7 @@
     </row>
     <row r="50" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -4323,7 +4298,7 @@
     </row>
     <row r="51" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -4336,7 +4311,7 @@
     </row>
     <row r="52" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A52" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -4349,7 +4324,7 @@
     </row>
     <row r="53" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -4362,7 +4337,7 @@
     </row>
     <row r="54" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A54" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -4375,7 +4350,7 @@
     </row>
     <row r="55" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A55" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -4388,7 +4363,7 @@
     </row>
     <row r="56" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -4401,7 +4376,7 @@
     </row>
     <row r="57" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A57" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -4414,7 +4389,7 @@
     </row>
     <row r="58" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A58" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -4427,7 +4402,7 @@
     </row>
     <row r="59" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A59" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -4440,7 +4415,7 @@
     </row>
     <row r="60" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A60" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -4453,13 +4428,13 @@
     </row>
     <row r="61" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A61" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1">
         <v>1</v>
@@ -4475,13 +4450,13 @@
     </row>
     <row r="62" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A62" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
@@ -4497,13 +4472,13 @@
     </row>
     <row r="63" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A63" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63" s="1">
         <v>1</v>
@@ -4519,13 +4494,13 @@
     </row>
     <row r="64" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A64" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E64" s="1">
         <v>1</v>
@@ -4541,13 +4516,13 @@
     </row>
     <row r="65" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A65" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -4563,13 +4538,13 @@
     </row>
     <row r="66" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A66" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E66" s="1">
         <v>1</v>
@@ -4585,13 +4560,13 @@
     </row>
     <row r="67" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A67" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67" s="1">
         <v>2</v>
@@ -4607,13 +4582,13 @@
     </row>
     <row r="68" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A68" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" s="1">
         <v>2</v>
@@ -4629,13 +4604,13 @@
     </row>
     <row r="69" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A69" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
@@ -4651,13 +4626,13 @@
     </row>
     <row r="70" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A70" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E70" s="1">
         <v>2</v>
@@ -4673,13 +4648,13 @@
     </row>
     <row r="71" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A71" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E71" s="1">
         <v>2</v>
@@ -4695,13 +4670,13 @@
     </row>
     <row r="72" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A72" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E72" s="1">
         <v>2</v>
@@ -4717,7 +4692,7 @@
     </row>
     <row r="73" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A73" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -4730,7 +4705,7 @@
     </row>
     <row r="74" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A74" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -4743,7 +4718,7 @@
     </row>
     <row r="75" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A75" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -4756,7 +4731,7 @@
     </row>
     <row r="76" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A76" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -4769,7 +4744,7 @@
     </row>
     <row r="77" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A77" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -4782,7 +4757,7 @@
     </row>
     <row r="78" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A78" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -4795,13 +4770,13 @@
     </row>
     <row r="79" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A79" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E79" s="1">
         <v>4</v>
@@ -4817,13 +4792,13 @@
     </row>
     <row r="80" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A80" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E80" s="1">
         <v>4</v>
@@ -4839,13 +4814,13 @@
     </row>
     <row r="81" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A81" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E81" s="1">
         <v>4</v>
@@ -4861,13 +4836,13 @@
     </row>
     <row r="82" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A82" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E82" s="1">
         <v>4</v>
@@ -4883,13 +4858,13 @@
     </row>
     <row r="83" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A83" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E83" s="1">
         <v>4</v>
@@ -4905,13 +4880,13 @@
     </row>
     <row r="84" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A84" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E84" s="1">
         <v>4</v>
@@ -4927,7 +4902,7 @@
     </row>
     <row r="85" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A85" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -4940,7 +4915,7 @@
     </row>
     <row r="86" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A86" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -4953,7 +4928,7 @@
     </row>
     <row r="87" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A87" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -4966,7 +4941,7 @@
     </row>
     <row r="88" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A88" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -4979,7 +4954,7 @@
     </row>
     <row r="89" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A89" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -4992,7 +4967,7 @@
     </row>
     <row r="90" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A90" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -5017,8 +4992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFBECD2-99BF-47E1-9785-39A18FE51D4F}">
   <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5031,7 +5006,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -5040,33 +5015,33 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1">
       <c r="A2" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -5079,7 +5054,7 @@
     </row>
     <row r="3" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -5092,7 +5067,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -5101,7 +5076,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K4" s="1"/>
     </row>
@@ -5110,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -5123,13 +5098,13 @@
     </row>
     <row r="6" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A6" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -5143,7 +5118,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -5152,19 +5127,19 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E8" s="1">
         <v>0</v>
@@ -5178,13 +5153,13 @@
     </row>
     <row r="9" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -5198,13 +5173,13 @@
     </row>
     <row r="10" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
@@ -5218,13 +5193,13 @@
     </row>
     <row r="11" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
@@ -5238,16 +5213,16 @@
     </row>
     <row r="12" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A12" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -5261,7 +5236,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="1"/>
@@ -5275,7 +5250,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="1"/>
@@ -5289,7 +5264,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A15" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="1"/>
@@ -5303,7 +5278,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1"/>
@@ -5317,10 +5292,10 @@
     </row>
     <row r="17" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -5336,7 +5311,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -5349,14 +5324,14 @@
     </row>
     <row r="19" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A19" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E19" s="1">
         <v>1</v>
@@ -5372,14 +5347,14 @@
     </row>
     <row r="20" spans="1:11" ht="13.95" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E20" s="1">
         <v>1</v>
@@ -5392,16 +5367,16 @@
     </row>
     <row r="21" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A21" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="1">
         <v>0</v>
@@ -5415,7 +5390,7 @@
     </row>
     <row r="22" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A22" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
@@ -5429,14 +5404,14 @@
     </row>
     <row r="23" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E23" s="1">
         <v>1</v>
@@ -5450,14 +5425,14 @@
     </row>
     <row r="24" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E24" s="1">
         <v>1</v>
@@ -5471,14 +5446,14 @@
     </row>
     <row r="25" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E25" s="1">
         <v>1</v>
@@ -5492,10 +5467,10 @@
     </row>
     <row r="26" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="1"/>
@@ -5509,7 +5484,7 @@
     </row>
     <row r="27" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
@@ -5523,7 +5498,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="1"/>
@@ -5537,19 +5512,19 @@
     </row>
     <row r="29" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G29" s="1">
         <v>0</v>
@@ -5561,19 +5536,19 @@
     </row>
     <row r="30" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E30" s="1">
         <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
@@ -5585,19 +5560,19 @@
     </row>
     <row r="31" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A31" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="1">
         <v>3</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
@@ -5609,7 +5584,7 @@
     </row>
     <row r="32" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A32" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -5622,7 +5597,7 @@
     </row>
     <row r="33" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -5635,7 +5610,7 @@
     </row>
     <row r="34" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A34" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -5648,7 +5623,7 @@
     </row>
     <row r="35" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A35" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -5661,7 +5636,7 @@
     </row>
     <row r="36" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A36" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -5674,7 +5649,7 @@
     </row>
     <row r="37" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A37" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -5687,7 +5662,7 @@
     </row>
     <row r="38" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A38" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -5700,7 +5675,7 @@
     </row>
     <row r="39" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A39" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -5713,7 +5688,7 @@
     </row>
     <row r="40" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A40" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -5726,19 +5701,19 @@
     </row>
     <row r="41" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A41" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G41" s="1">
         <v>0</v>
@@ -5750,7 +5725,7 @@
     </row>
     <row r="42" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A42" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -5763,19 +5738,19 @@
     </row>
     <row r="43" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E43" s="1">
         <v>3</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
@@ -5787,7 +5762,7 @@
     </row>
     <row r="44" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A44" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -5800,7 +5775,7 @@
     </row>
     <row r="45" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A45" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -5813,7 +5788,7 @@
     </row>
     <row r="46" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A46" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -5826,19 +5801,19 @@
     </row>
     <row r="47" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A47" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E47" s="1">
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -5850,7 +5825,7 @@
     </row>
     <row r="48" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A48" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -5863,19 +5838,19 @@
     </row>
     <row r="49" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A49" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E49" s="1">
         <v>3</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -5887,7 +5862,7 @@
     </row>
     <row r="50" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A50" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -5900,7 +5875,7 @@
     </row>
     <row r="51" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A51" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -5913,7 +5888,7 @@
     </row>
     <row r="52" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A52" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -5926,7 +5901,7 @@
     </row>
     <row r="53" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A53" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -5939,7 +5914,7 @@
     </row>
     <row r="54" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A54" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -5952,7 +5927,7 @@
     </row>
     <row r="55" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A55" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -5965,7 +5940,7 @@
     </row>
     <row r="56" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -5978,7 +5953,7 @@
     </row>
     <row r="57" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A57" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -5991,7 +5966,7 @@
     </row>
     <row r="58" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A58" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -6004,7 +5979,7 @@
     </row>
     <row r="59" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A59" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -6017,7 +5992,7 @@
     </row>
     <row r="60" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A60" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -6030,19 +6005,19 @@
     </row>
     <row r="61" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A61" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E61" s="1">
         <v>0</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
@@ -6054,19 +6029,19 @@
     </row>
     <row r="62" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A62" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62" s="1">
         <v>1</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G62" s="1">
         <v>0</v>
@@ -6078,19 +6053,19 @@
     </row>
     <row r="63" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A63" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E63" s="1">
         <v>2</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
@@ -6102,7 +6077,7 @@
     </row>
     <row r="64" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A64" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -6115,7 +6090,7 @@
     </row>
     <row r="65" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A65" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -6128,7 +6103,7 @@
     </row>
     <row r="66" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A66" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -6141,19 +6116,19 @@
     </row>
     <row r="67" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A67" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E67" s="1">
         <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
@@ -6165,19 +6140,19 @@
     </row>
     <row r="68" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A68" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E68" s="1">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -6189,19 +6164,19 @@
     </row>
     <row r="69" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A69" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E69" s="1">
         <v>2</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -6213,7 +6188,7 @@
     </row>
     <row r="70" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A70" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -6226,7 +6201,7 @@
     </row>
     <row r="71" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A71" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -6239,7 +6214,7 @@
     </row>
     <row r="72" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A72" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -6252,7 +6227,7 @@
     </row>
     <row r="73" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A73" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -6265,7 +6240,7 @@
     </row>
     <row r="74" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A74" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -6278,7 +6253,7 @@
     </row>
     <row r="75" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A75" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -6291,7 +6266,7 @@
     </row>
     <row r="76" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A76" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -6304,7 +6279,7 @@
     </row>
     <row r="77" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A77" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -6317,7 +6292,7 @@
     </row>
     <row r="78" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A78" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -6330,7 +6305,7 @@
     </row>
     <row r="79" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A79" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -6343,7 +6318,7 @@
     </row>
     <row r="80" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A80" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -6356,7 +6331,7 @@
     </row>
     <row r="81" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A81" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -6369,7 +6344,7 @@
     </row>
     <row r="82" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A82" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -6382,7 +6357,7 @@
     </row>
     <row r="83" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A83" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -6395,7 +6370,7 @@
     </row>
     <row r="84" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A84" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -6408,7 +6383,7 @@
     </row>
     <row r="85" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A85" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -6421,7 +6396,7 @@
     </row>
     <row r="86" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A86" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -6434,7 +6409,7 @@
     </row>
     <row r="87" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A87" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -6447,7 +6422,7 @@
     </row>
     <row r="88" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A88" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -6460,7 +6435,7 @@
     </row>
     <row r="89" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A89" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -6473,7 +6448,7 @@
     </row>
     <row r="90" spans="1:11" ht="15.6" thickTop="1" thickBot="1">
       <c r="A90" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>

</xml_diff>